<commit_message>
edited other control csv's to match what I got working with batch1
</commit_message>
<xml_diff>
--- a/control4.xlsx
+++ b/control4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenzieobrien/mlc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74593CF4-4861-604D-A13B-AF8ED00E8D40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44A4372-AFA8-6C46-ABDF-C06971CA6BE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15180" xr2:uid="{80DAE7BE-0E0B-DE4D-B4BF-A571C76BE4A2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="55">
   <si>
     <t>crunchy, chewy</t>
   </si>
@@ -169,6 +169,33 @@
   </si>
   <si>
     <t>Jackson.klarsfeld1@marist.edu</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>aroma</t>
+  </si>
+  <si>
+    <t>taste</t>
+  </si>
+  <si>
+    <t>texture</t>
+  </si>
+  <si>
+    <t>overall_sat</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sendEmail</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -527,70 +554,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1A1502-E58A-C24D-8A66-5ACC422A58D9}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
@@ -610,25 +631,25 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -651,19 +672,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>4</v>
@@ -677,25 +698,25 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>3</v>
@@ -712,22 +733,22 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>2</v>
@@ -747,7 +768,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>4</v>
@@ -756,13 +777,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>2</v>
@@ -782,22 +803,22 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
@@ -810,29 +831,25 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
@@ -852,13 +869,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -867,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>2</v>
@@ -890,19 +907,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>2</v>
@@ -925,19 +942,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>2</v>
@@ -957,7 +974,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
@@ -966,16 +983,16 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>3</v>
@@ -992,22 +1009,22 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
@@ -1027,25 +1044,25 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>3</v>
@@ -1071,19 +1088,19 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>4</v>
@@ -1103,25 +1120,25 @@
         <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1132,31 +1149,31 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1167,7 +1184,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
@@ -1182,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>2</v>
@@ -1202,22 +1219,22 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>2</v>
@@ -1237,7 +1254,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -1246,16 +1263,16 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
@@ -1278,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>0</v>
@@ -1287,10 +1304,10 @@
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>10</v>
@@ -1307,31 +1324,31 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1345,28 +1362,28 @@
         <v>5</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1380,25 +1397,25 @@
         <v>5</v>
       </c>
       <c r="B25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1">
         <v>9</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>4</v>
@@ -1412,25 +1429,25 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>10</v>
@@ -1447,28 +1464,28 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1">
         <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="1">
         <v>8</v>
       </c>
-      <c r="E27" s="1">
-        <v>7</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>4</v>
@@ -1494,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>7</v>
@@ -1529,10 +1546,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
@@ -1552,10 +1569,10 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1">
         <v>5</v>
@@ -1564,13 +1581,13 @@
         <v>8</v>
       </c>
       <c r="E30" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>3</v>
@@ -1587,28 +1604,28 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1">
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>4</v>
@@ -1622,31 +1639,31 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1657,31 +1674,31 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
       </c>
       <c r="C33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1692,28 +1709,28 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B34" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
         <v>6</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>4</v>
@@ -1725,6 +1742,41 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>